<commit_message>
refactor George's classifier factory out of experiments
</commit_message>
<xml_diff>
--- a/docs/Dependency Map.xlsx
+++ b/docs/Dependency Map.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>jar</t>
   </si>
@@ -126,19 +126,28 @@
   </si>
   <si>
     <t>TSCHIEFWrapper</t>
+  </si>
+  <si>
+    <t>ResultsProcessing?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -161,8 +170,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +458,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,6 +563,12 @@
       <c r="A15" t="s">
         <v>15</v>
       </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -614,9 +632,13 @@
       <c r="A24" t="s">
         <v>24</v>
       </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>